<commit_message>
TCC Trabalho Escrito - Rev1
</commit_message>
<xml_diff>
--- a/Resultado_Neural_Networks.xlsx
+++ b/Resultado_Neural_Networks.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Resultados" sheetId="1" r:id="rId1"/>
+    <sheet name="Plan1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="15">
   <si>
     <t>lista_funcao_ativacao</t>
   </si>
@@ -36,18 +37,48 @@
   <si>
     <t>-</t>
   </si>
+  <si>
+    <t>Função de Ativação</t>
+  </si>
+  <si>
+    <t>Sigmóide</t>
+  </si>
+  <si>
+    <t>Softplus</t>
+  </si>
+  <si>
+    <t>ReLu</t>
+  </si>
+  <si>
+    <t>Quatidade de Camadas</t>
+  </si>
+  <si>
+    <t>Quantidade de Neurônios</t>
+  </si>
+  <si>
+    <t>Resultado - MSE</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -64,7 +95,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -72,11 +103,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -85,6 +127,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -382,9 +432,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomLeft" sqref="A1:E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,4 +1034,431 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F28"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5">
+        <v>5</v>
+      </c>
+      <c r="D2" s="5">
+        <v>1.1691510000000001</v>
+      </c>
+      <c r="F2">
+        <f>MIN(D2:D28)</f>
+        <v>1.1558250000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5">
+        <v>10</v>
+      </c>
+      <c r="D3" s="5">
+        <v>1.173829</v>
+      </c>
+      <c r="F3">
+        <v>1.1558250000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="5">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5">
+        <v>15</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1.2124980000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="5">
+        <v>5</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1.1724950000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="5">
+        <v>2</v>
+      </c>
+      <c r="C6" s="5">
+        <v>10</v>
+      </c>
+      <c r="D6" s="5">
+        <v>1.2042280000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="5">
+        <v>2</v>
+      </c>
+      <c r="C7" s="5">
+        <v>15</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1.3273680000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="5">
+        <v>3</v>
+      </c>
+      <c r="C8" s="5">
+        <v>5</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1.167605</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5">
+        <v>3</v>
+      </c>
+      <c r="C9" s="5">
+        <v>10</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1.2266950000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5">
+        <v>3</v>
+      </c>
+      <c r="C10" s="5">
+        <v>15</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1.3719159999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="5">
+        <v>1</v>
+      </c>
+      <c r="C11" s="5">
+        <v>5</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1.1558250000000001</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="5">
+        <v>1</v>
+      </c>
+      <c r="C12" s="5">
+        <v>10</v>
+      </c>
+      <c r="D12" s="5">
+        <v>1.1991810000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="5">
+        <v>1</v>
+      </c>
+      <c r="C13" s="5">
+        <v>15</v>
+      </c>
+      <c r="D13" s="5">
+        <v>1.189762</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="5">
+        <v>2</v>
+      </c>
+      <c r="C14" s="5">
+        <v>5</v>
+      </c>
+      <c r="D14" s="5">
+        <v>1.176706</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="5">
+        <v>2</v>
+      </c>
+      <c r="C15" s="5">
+        <v>10</v>
+      </c>
+      <c r="D15" s="5">
+        <v>8.310981</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="5">
+        <v>2</v>
+      </c>
+      <c r="C16" s="5">
+        <v>15</v>
+      </c>
+      <c r="D16" s="5">
+        <v>2.5078809999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="5">
+        <v>3</v>
+      </c>
+      <c r="C17" s="5">
+        <v>5</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="5">
+        <v>3</v>
+      </c>
+      <c r="C18" s="5">
+        <v>10</v>
+      </c>
+      <c r="D18" s="5">
+        <v>3.1337290000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="5">
+        <v>3</v>
+      </c>
+      <c r="C19" s="5">
+        <v>15</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="5">
+        <v>1</v>
+      </c>
+      <c r="C20" s="5">
+        <v>5</v>
+      </c>
+      <c r="D20" s="5">
+        <v>2.3436880000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="5">
+        <v>1</v>
+      </c>
+      <c r="C21" s="5">
+        <v>10</v>
+      </c>
+      <c r="D21" s="5">
+        <v>2.6155949999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="5">
+        <v>1</v>
+      </c>
+      <c r="C22" s="5">
+        <v>15</v>
+      </c>
+      <c r="D22" s="5">
+        <v>2.810168</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="5">
+        <v>2</v>
+      </c>
+      <c r="C23" s="5">
+        <v>5</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="5">
+        <v>2</v>
+      </c>
+      <c r="C24" s="5">
+        <v>10</v>
+      </c>
+      <c r="D24" s="5">
+        <v>2.8101820000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="5">
+        <v>2</v>
+      </c>
+      <c r="C25" s="5">
+        <v>15</v>
+      </c>
+      <c r="D25" s="5">
+        <v>2.810168</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="5">
+        <v>3</v>
+      </c>
+      <c r="C26" s="5">
+        <v>5</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="5">
+        <v>3</v>
+      </c>
+      <c r="C27" s="5">
+        <v>10</v>
+      </c>
+      <c r="D27" s="5">
+        <v>2.810168</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="5">
+        <v>3</v>
+      </c>
+      <c r="C28" s="5">
+        <v>15</v>
+      </c>
+      <c r="D28" s="5">
+        <v>2.810168</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>